<commit_message>
fix done with new version
</commit_message>
<xml_diff>
--- a/DE_XUAT_VAT_TU_NGHIEN_CUU_BO_DIEU_KHIEN_MAY_BAY_DOT_3.xlsx
+++ b/DE_XUAT_VAT_TU_NGHIEN_CUU_BO_DIEU_KHIEN_MAY_BAY_DOT_3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="20655" yWindow="345" windowWidth="14805" windowHeight="7770"/>
+    <workbookView xWindow="23244" yWindow="348" windowWidth="14808" windowHeight="7776"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="71">
   <si>
     <t>TẬP ĐOÀN VDI GROUP</t>
   </si>
@@ -231,12 +231,6 @@
     <t>https://shopee.vn/-Sa%CC%A3c-Nhanh-D%C3%A2y-sa%CC%A3c-samsung-oppo-xiaomi...-C%C3%A1p-s%E1%BA%A1c-c%E1%BB%95ng-Micro-USB-thi%E1%BA%BFt-k%E1%BA%BF-d%C3%A2y-b%E1%BB%87n-du%CC%80-cho-%C4%91i%E1%BB%87n-tho%E1%BA%A1i-androi-i.223789752.5564849127?position=28</t>
   </si>
   <si>
-    <t>Mạch in v1</t>
-  </si>
-  <si>
-    <t>Mạch in v2</t>
-  </si>
-  <si>
     <t>https://cxt.vn/</t>
   </si>
   <si>
@@ -246,6 +240,15 @@
   </si>
   <si>
     <t>Hàn + Khò DeBaiLong 8786D</t>
+  </si>
+  <si>
+    <t>&lt;20 ngày</t>
+  </si>
+  <si>
+    <t>Mạch in ina_board_1</t>
+  </si>
+  <si>
+    <t>Mạch in ina_board_2</t>
   </si>
 </sst>
 </file>
@@ -832,23 +835,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" customWidth="1"/>
     <col min="8" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C1" s="18" t="s">
         <v>0</v>
       </c>
@@ -860,12 +863,12 @@
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="20"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="22"/>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -885,7 +888,7 @@
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
     </row>
-    <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D5" s="24" t="s">
         <v>20</v>
       </c>
@@ -893,9 +896,9 @@
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
     </row>
-    <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -906,7 +909,7 @@
       <c r="I6" s="26"/>
       <c r="J6" s="26"/>
     </row>
-    <row r="7" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
@@ -938,7 +941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>1</v>
       </c>
@@ -966,7 +969,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>2</v>
       </c>
@@ -994,7 +997,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>3</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14">
         <v>4</v>
       </c>
@@ -1050,7 +1053,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14">
         <v>5</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
         <v>6</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14">
         <v>7</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14">
         <v>8</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
         <v>9</v>
       </c>
@@ -1190,12 +1193,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14">
         <v>10</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
@@ -1218,7 +1221,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14">
         <v>11</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14">
         <v>12</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14">
         <v>13</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14">
         <v>14</v>
       </c>
@@ -1330,7 +1333,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14">
         <v>15</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="14">
         <v>16</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14">
         <v>17</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14">
         <v>18</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14">
         <v>19</v>
       </c>
@@ -1473,12 +1476,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14">
         <v>20</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -1492,21 +1495,21 @@
         <v>17</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>23</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="14">
         <v>21</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
@@ -1520,16 +1523,16 @@
         <v>17</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>23</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="27" t="s">
         <v>19</v>
       </c>
@@ -1542,7 +1545,7 @@
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
     </row>
-    <row r="30" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1555,7 +1558,7 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
     </row>
-    <row r="32" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B32" s="19" t="s">
         <v>11</v>
       </c>
@@ -1572,7 +1575,7 @@
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
     </row>
-    <row r="33" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1582,7 +1585,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1592,7 +1595,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1602,7 +1605,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1612,7 +1615,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1622,7 +1625,7 @@
       <c r="I37" s="8"/>
       <c r="J37" s="9"/>
     </row>
-    <row r="38" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B38" s="19" t="s">
         <v>13</v>
       </c>

</xml_diff>